<commit_message>
Últimas alterações da versão 1
</commit_message>
<xml_diff>
--- a/docs/Product Backlog.xlsx
+++ b/docs/Product Backlog.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djsla\OneDrive\Ambiente de Trabalho\picand-go\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LUÍS PEREIRA\GitHub\picand-go\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA7792F-7D4E-47E8-BFB8-807DCD090124}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A4AA5B-D980-4D63-9A2C-4D0CE50AD45B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="-120" windowWidth="19740" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tarefas" sheetId="5" r:id="rId1"/>
+    <sheet name="Requisitos" sheetId="5" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -147,9 +147,6 @@
     <t>ID do Requisito</t>
   </si>
   <si>
-    <t>Coluna1</t>
-  </si>
-  <si>
     <t>Funcional</t>
   </si>
   <si>
@@ -460,6 +457,9 @@
   </si>
   <si>
     <t>R-055</t>
+  </si>
+  <si>
+    <t>Tipo</t>
   </si>
 </sst>
 </file>
@@ -584,1536 +584,6 @@
   <dxfs count="169">
     <dxf>
       <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF639AF2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFBE5BE3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDB6B46"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2130,7 +600,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2150,7 +620,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2210,7 +680,7 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2230,7 +700,8 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="164" formatCode="&quot;Por Fazer&quot;;&quot;Feito&quot;"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2310,7 +781,6 @@
         <charset val="1"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="164" formatCode="&quot;Por Fazer&quot;;&quot;Feito&quot;"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2438,6 +908,1536 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF639AF2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFBE5BE3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDB6B46"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2533,16 +2533,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1198A39D-FAF6-4CC2-BC9B-BD1DFBB184C3}" name="Tabela_Requisitos" displayName="Tabela_Requisitos" ref="A2:G288" headerRowDxfId="168" dataDxfId="167">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1198A39D-FAF6-4CC2-BC9B-BD1DFBB184C3}" name="Tabela_Requisitos" displayName="Tabela_Requisitos" ref="A2:G288" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="A2:G288" xr:uid="{FA7D6100-5CD1-494D-A60D-8E892EAEC05C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3FC58B53-8DA1-4447-BCED-3625FD40251E}" name="ID do Requisito" totalsRowLabel="Total" dataDxfId="166" totalsRowDxfId="165"/>
-    <tableColumn id="2" xr3:uid="{1FECF677-DAA3-4088-BB5D-F7B8E4CC16B8}" name="Coluna1" dataDxfId="155" totalsRowDxfId="156"/>
-    <tableColumn id="6" xr3:uid="{DC30BE9F-8023-4604-87CE-B0741D99D9E9}" name="Nome" dataDxfId="153" totalsRowDxfId="154"/>
-    <tableColumn id="3" xr3:uid="{BFBE8AC3-C050-4F78-8B7C-E36215B1671A}" name="Descrição" dataDxfId="164" totalsRowDxfId="163"/>
-    <tableColumn id="4" xr3:uid="{47565725-4927-48A7-90AA-0A8734EA4A8A}" name="Status" dataDxfId="162" totalsRowDxfId="161"/>
-    <tableColumn id="5" xr3:uid="{32A88ECC-C6F1-4077-B4ED-D92962146243}" name="Responsável" dataDxfId="160" totalsRowDxfId="159"/>
-    <tableColumn id="7" xr3:uid="{1E911A97-3917-4ACE-B36D-84BA008FE615}" name="Prioridade" totalsRowFunction="count" dataDxfId="158" totalsRowDxfId="157"/>
+    <tableColumn id="1" xr3:uid="{3FC58B53-8DA1-4447-BCED-3625FD40251E}" name="ID do Requisito" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{1FECF677-DAA3-4088-BB5D-F7B8E4CC16B8}" name="Tipo" dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{DC30BE9F-8023-4604-87CE-B0741D99D9E9}" name="Nome" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{BFBE8AC3-C050-4F78-8B7C-E36215B1671A}" name="Descrição" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{47565725-4927-48A7-90AA-0A8734EA4A8A}" name="Status" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{32A88ECC-C6F1-4077-B4ED-D92962146243}" name="Responsável" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{1E911A97-3917-4ACE-B36D-84BA008FE615}" name="Prioridade" totalsRowFunction="count" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2847,8 +2847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{925233BC-DEF4-4153-A45F-C1645D7758F5}">
   <dimension ref="A1:G288"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40:F48"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2877,13 +2877,13 @@
         <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>141</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>6</v>
@@ -2900,13 +2900,13 @@
         <v>13</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>9</v>
@@ -2923,13 +2923,13 @@
         <v>14</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>9</v>
@@ -2946,13 +2946,13 @@
         <v>15</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>9</v>
@@ -2969,13 +2969,13 @@
         <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>9</v>
@@ -2992,13 +2992,13 @@
         <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>9</v>
@@ -3015,13 +3015,13 @@
         <v>18</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>9</v>
@@ -3038,13 +3038,13 @@
         <v>19</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>9</v>
@@ -3061,13 +3061,13 @@
         <v>20</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E10" s="5" t="s">
         <v>9</v>
@@ -3084,13 +3084,13 @@
         <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>9</v>
@@ -3107,13 +3107,13 @@
         <v>22</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>9</v>
@@ -3130,13 +3130,13 @@
         <v>23</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>9</v>
@@ -3153,13 +3153,13 @@
         <v>24</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>9</v>
@@ -3176,13 +3176,13 @@
         <v>25</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>9</v>
@@ -3199,13 +3199,13 @@
         <v>26</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>9</v>
@@ -3222,13 +3222,13 @@
         <v>27</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>9</v>
@@ -3245,13 +3245,13 @@
         <v>28</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>9</v>
@@ -3268,13 +3268,13 @@
         <v>29</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>9</v>
@@ -3291,13 +3291,13 @@
         <v>30</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>9</v>
@@ -3314,13 +3314,13 @@
         <v>31</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" s="5" t="s">
         <v>9</v>
@@ -3337,13 +3337,13 @@
         <v>32</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E22" s="5" t="s">
         <v>9</v>
@@ -3360,13 +3360,13 @@
         <v>33</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>9</v>
@@ -3383,13 +3383,13 @@
         <v>34</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>9</v>
@@ -3406,13 +3406,13 @@
         <v>35</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>9</v>
@@ -3426,16 +3426,16 @@
     </row>
     <row r="26" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>9</v>
@@ -3449,16 +3449,16 @@
     </row>
     <row r="27" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>9</v>
@@ -3472,16 +3472,16 @@
     </row>
     <row r="28" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>9</v>
@@ -3495,16 +3495,16 @@
     </row>
     <row r="29" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>9</v>
@@ -3518,16 +3518,16 @@
     </row>
     <row r="30" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>9</v>
@@ -3541,16 +3541,16 @@
     </row>
     <row r="31" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>9</v>
@@ -3564,16 +3564,16 @@
     </row>
     <row r="32" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>9</v>
@@ -3587,16 +3587,16 @@
     </row>
     <row r="33" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>9</v>
@@ -3610,16 +3610,16 @@
     </row>
     <row r="34" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>9</v>
@@ -3633,16 +3633,16 @@
     </row>
     <row r="35" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>9</v>
@@ -3656,16 +3656,16 @@
     </row>
     <row r="36" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>9</v>
@@ -3679,16 +3679,16 @@
     </row>
     <row r="37" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>9</v>
@@ -3702,16 +3702,16 @@
     </row>
     <row r="38" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E38" s="5" t="s">
         <v>9</v>
@@ -3725,16 +3725,16 @@
     </row>
     <row r="39" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>9</v>
@@ -3748,16 +3748,16 @@
     </row>
     <row r="40" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E40" s="5" t="s">
         <v>9</v>
@@ -3771,16 +3771,16 @@
     </row>
     <row r="41" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E41" s="5" t="s">
         <v>9</v>
@@ -3794,16 +3794,16 @@
     </row>
     <row r="42" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>9</v>
@@ -3817,16 +3817,16 @@
     </row>
     <row r="43" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E43" s="5" t="s">
         <v>9</v>
@@ -3840,16 +3840,16 @@
     </row>
     <row r="44" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E44" s="5" t="s">
         <v>9</v>
@@ -3863,16 +3863,16 @@
     </row>
     <row r="45" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E45" s="5" t="s">
         <v>9</v>
@@ -3886,16 +3886,16 @@
     </row>
     <row r="46" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>9</v>
@@ -3909,16 +3909,16 @@
     </row>
     <row r="47" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>9</v>
@@ -3932,16 +3932,16 @@
     </row>
     <row r="48" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E48" s="5" t="s">
         <v>9</v>
@@ -6116,13 +6116,13 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="G67:G132 G135:G173 G175:G187 G189:G288 G3:G45">
-    <cfRule type="cellIs" dxfId="152" priority="353" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="353" operator="equal">
       <formula>"Baixa"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="358" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="358" operator="equal">
       <formula>"Média"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="150" priority="359" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="359" operator="equal">
       <formula>"Alta"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6145,13 +6145,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46">
-    <cfRule type="cellIs" dxfId="149" priority="296" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="296" operator="equal">
       <formula>"Baixa"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="297" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="297" operator="equal">
       <formula>"Média"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="147" priority="298" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="298" operator="equal">
       <formula>"Alta"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6172,24 +6172,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47">
-    <cfRule type="cellIs" dxfId="146" priority="307" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="307" operator="equal">
       <formula>"Baixa"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="308" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="308" operator="equal">
       <formula>"Média"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="144" priority="309" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="309" operator="equal">
       <formula>"Alta"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G48:G96">
-    <cfRule type="cellIs" dxfId="143" priority="304" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="304" operator="equal">
       <formula>"Baixa"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="305" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="305" operator="equal">
       <formula>"Média"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="141" priority="306" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="306" operator="equal">
       <formula>"Alta"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6274,24 +6274,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G133">
-    <cfRule type="cellIs" dxfId="140" priority="246" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="246" operator="equal">
       <formula>"Baixa"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="247" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="247" operator="equal">
       <formula>"Média"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="138" priority="248" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="248" operator="equal">
       <formula>"Alta"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G134">
-    <cfRule type="cellIs" dxfId="137" priority="243" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="243" operator="equal">
       <formula>"Baixa"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="244" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="244" operator="equal">
       <formula>"Média"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="245" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="245" operator="equal">
       <formula>"Alta"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6472,24 +6472,24 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G174">
-    <cfRule type="cellIs" dxfId="134" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="213" operator="equal">
       <formula>"Baixa"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="214" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="214" operator="equal">
       <formula>"Média"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="215" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="215" operator="equal">
       <formula>"Alta"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G188">
-    <cfRule type="cellIs" dxfId="131" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="210" operator="equal">
       <formula>"Baixa"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="211" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="211" operator="equal">
       <formula>"Média"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="212" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="212" operator="equal">
       <formula>"Alta"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6510,475 +6510,475 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B246:C251 C40:C44">
-    <cfRule type="containsText" dxfId="128" priority="207" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="144" priority="207" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="208" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="143" priority="208" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B40)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="209" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="142" priority="209" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B40)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B288:C288">
-    <cfRule type="containsText" dxfId="125" priority="138" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="141" priority="138" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B288)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="139" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="140" priority="139" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B288)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="140" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="139" priority="140" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B288)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B49:C71 C48">
-    <cfRule type="containsText" dxfId="122" priority="195" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="138" priority="195" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="196" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="137" priority="196" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="197" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="136" priority="197" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B73:C99">
-    <cfRule type="containsText" dxfId="119" priority="192" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="135" priority="192" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="193" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="134" priority="193" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B73)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="194" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="133" priority="194" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B100:C132">
-    <cfRule type="containsText" dxfId="116" priority="189" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="132" priority="189" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="190" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="131" priority="190" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="191" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="130" priority="191" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B100)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B133:C164">
-    <cfRule type="containsText" dxfId="113" priority="186" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="129" priority="186" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B133)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="187" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="128" priority="187" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B133)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="188" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="127" priority="188" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B133)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B165:C202">
-    <cfRule type="containsText" dxfId="110" priority="183" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="126" priority="183" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B165)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="184" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="125" priority="184" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B165)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="185" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="124" priority="185" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B165)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C47">
-    <cfRule type="containsText" dxfId="107" priority="150" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="123" priority="150" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",C47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="151" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="122" priority="151" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",C47)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="152" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="121" priority="152" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",C47)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="containsText" dxfId="104" priority="147" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="120" priority="147" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",C46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="148" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="119" priority="148" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",C46)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="149" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="118" priority="149" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",C46)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C45">
-    <cfRule type="containsText" dxfId="101" priority="144" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="117" priority="144" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",C45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="145" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="116" priority="145" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",C45)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="146" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="115" priority="146" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",C45)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72:C72">
-    <cfRule type="containsText" dxfId="98" priority="141" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="114" priority="141" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B72)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="142" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="113" priority="142" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B72)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="143" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="112" priority="143" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B203:C203">
-    <cfRule type="containsText" dxfId="95" priority="125" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="111" priority="125" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B203)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="126" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="110" priority="126" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B203)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="127" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="109" priority="127" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B203)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B204:C204">
-    <cfRule type="containsText" dxfId="92" priority="122" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="108" priority="122" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B204)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="123" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="107" priority="123" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B204)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="124" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="106" priority="124" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B204)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B205:C205">
-    <cfRule type="containsText" dxfId="89" priority="119" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="105" priority="119" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B205)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="120" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="104" priority="120" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B205)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="121" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="103" priority="121" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B205)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B206:C206">
-    <cfRule type="containsText" dxfId="86" priority="116" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="102" priority="116" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B206)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="117" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="101" priority="117" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B206)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="118" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="100" priority="118" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B206)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B207:C207">
-    <cfRule type="containsText" dxfId="83" priority="113" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="99" priority="113" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B207)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="114" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="98" priority="114" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B207)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="115" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="97" priority="115" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B207)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B208:C212">
-    <cfRule type="containsText" dxfId="80" priority="110" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="96" priority="110" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B208)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="111" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="95" priority="111" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B208)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="112" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="94" priority="112" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B208)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B213:C213">
-    <cfRule type="containsText" dxfId="77" priority="107" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="93" priority="107" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B213)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="108" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="92" priority="108" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B213)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="109" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="91" priority="109" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B213)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B214:C216 B219:C220">
-    <cfRule type="containsText" dxfId="74" priority="101" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="90" priority="101" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B214)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="102" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="89" priority="102" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B214)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="103" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="88" priority="103" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B214)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B237:C237">
-    <cfRule type="containsText" dxfId="71" priority="95" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="87" priority="95" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B237)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="96" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="86" priority="96" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B237)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="97" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="85" priority="97" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B237)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B245:C245">
-    <cfRule type="containsText" dxfId="68" priority="92" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="84" priority="92" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B245)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="93" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="83" priority="93" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B245)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="94" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="82" priority="94" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B245)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B244:C244">
-    <cfRule type="containsText" dxfId="65" priority="89" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="81" priority="89" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B244)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="90" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="80" priority="90" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B244)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="91" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="79" priority="91" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B244)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B236:C236">
-    <cfRule type="containsText" dxfId="62" priority="86" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="78" priority="86" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B236)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="87" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="77" priority="87" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B236)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="88" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="76" priority="88" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B236)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B235:C235">
-    <cfRule type="containsText" dxfId="59" priority="83" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="75" priority="83" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B235)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="84" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="74" priority="84" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B235)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="85" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="73" priority="85" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B235)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B234:C234">
-    <cfRule type="containsText" dxfId="56" priority="80" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="72" priority="80" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B234)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="81" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="71" priority="81" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B234)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="82" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="70" priority="82" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B234)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B242:C242">
-    <cfRule type="containsText" dxfId="53" priority="44" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="69" priority="44" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B242)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="45" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="68" priority="45" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B242)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="46" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="67" priority="46" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B242)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B231:C231">
-    <cfRule type="containsText" dxfId="50" priority="71" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="66" priority="71" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B231)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="72" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="65" priority="72" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B231)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="73" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="64" priority="73" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B231)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B229:C229">
-    <cfRule type="containsText" dxfId="47" priority="65" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="63" priority="65" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B229)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="66" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="62" priority="66" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B229)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="67" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="61" priority="67" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B229)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B228:C228">
-    <cfRule type="containsText" dxfId="44" priority="62" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="60" priority="62" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B228)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="63" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="59" priority="63" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B228)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="64" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="58" priority="64" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B228)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B243:C243">
-    <cfRule type="containsText" dxfId="41" priority="47" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="57" priority="47" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B243)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="48" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="56" priority="48" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B243)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="49" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="55" priority="49" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B243)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B240:C240">
-    <cfRule type="containsText" dxfId="38" priority="41" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="54" priority="41" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B240)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="42" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="53" priority="42" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B240)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="43" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="52" priority="43" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B240)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B227:C227">
-    <cfRule type="containsText" dxfId="35" priority="2" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="51" priority="2" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B227)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="3" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="50" priority="3" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B227)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="4" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="49" priority="4" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B227)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B241:C241">
-    <cfRule type="containsText" dxfId="32" priority="38" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="48" priority="38" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B241)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="39" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="47" priority="39" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B241)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="40" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="46" priority="40" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B241)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B239:C239">
-    <cfRule type="containsText" dxfId="29" priority="35" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="45" priority="35" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B239)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="36" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="44" priority="36" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B239)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="37" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="43" priority="37" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B239)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B238:C238">
-    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="42" priority="32" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B238)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="33" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="41" priority="33" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B238)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="34" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="40" priority="34" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B238)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B232:C232">
-    <cfRule type="containsText" dxfId="23" priority="29" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="39" priority="29" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B232)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="30" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="38" priority="30" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B232)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="31" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="37" priority="31" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B232)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B233:C233">
-    <cfRule type="containsText" dxfId="20" priority="26" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="36" priority="26" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B233)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="27" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="35" priority="27" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B233)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="28" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="34" priority="28" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B233)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B230:C230">
-    <cfRule type="containsText" dxfId="17" priority="23" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="33" priority="23" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B230)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="24" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="32" priority="24" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B230)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="25" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="31" priority="25" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B230)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B218:C218">
-    <cfRule type="containsText" dxfId="14" priority="20" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="30" priority="20" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B218)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="21" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="29" priority="21" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B218)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="22" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="28" priority="22" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B218)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B217:C217">
-    <cfRule type="containsText" dxfId="11" priority="17" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="27" priority="17" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B217)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="18" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="26" priority="18" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B217)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="19" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="25" priority="19" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B217)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B221:C221">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="24" priority="8" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B221)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="23" priority="9" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B221)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="22" priority="10" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B221)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B222:C222">
-    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="21" priority="11" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B222)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="12" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="20" priority="12" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B222)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="13" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B222)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B223:C226">
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Docs">
+    <cfRule type="containsText" dxfId="18" priority="5" operator="containsText" text="Docs">
       <formula>NOT(ISERROR(SEARCH("Docs",B223)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="Back-end">
+    <cfRule type="containsText" dxfId="17" priority="6" operator="containsText" text="Back-end">
       <formula>NOT(ISERROR(SEARCH("Back-end",B223)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="Front-end">
+    <cfRule type="containsText" dxfId="16" priority="7" operator="containsText" text="Front-end">
       <formula>NOT(ISERROR(SEARCH("Front-end",B223)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>